<commit_message>
Supported reading text tables
</commit_message>
<xml_diff>
--- a/data/Character.xlsx
+++ b/data/Character.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\GenshinSim\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBE72C2-FD3A-433E-90C5-326A888170A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C8C27F-6EBF-434F-8886-1921F4FA1C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,17 +17,26 @@
     <sheet name="CharacterTalentDataTable" sheetId="3" r:id="rId2"/>
     <sheet name="CharacterTalentEffectDataTable" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>### TABLE_TYPE</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -131,32 +140,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>普通攻击·西风剑术·宗室</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>普通攻击
-进行至多五段的连续挥砍。
-重击
-持续消耗体力，快速进行连续的斩击。
-重击结束时，会进行一次格外有力的挥砍。
-下落攻击从空中下坠冲击地面，攻击下落路径上的敌人，并在落地时造成范围伤害。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Texts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一段伤害;{0},
-二段伤害;{1},
-三段伤害;{2}+{2},
-四段伤害;{3},
-五段伤害;{4}+{4},
-重击循环伤害;{5},
-重击终结伤害;{6},
-下坠期间伤害;{7},
-低空/高空坠地冲击伤害;{8}/{9}</t>
+    <t>EffectTexts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skill.Common.SkillDamage1;{0},
+Skill.Common.SkillDamage2;{1},
+Skill.Common.SkillDamage3;{2}+{2},
+Skill.Common.SkillDamage4;{3},
+Skill.Common.SkillDamage5;{4}+{4},
+Skill.Common.ChargedAttackLoopDamage;{5},
+Skill.Common.ChargedAttackFinalDamage;{6},
+Skill.Common.PlungeDamage;{7},
+Skill.Common.LowHighPlungeDamage;{8}/{9}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -500,7 +496,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -546,7 +542,7 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -555,8 +551,8 @@
     <col min="2" max="2" width="14.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="67.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="27.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="80.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="72.375" style="2" customWidth="1"/>
     <col min="7" max="10" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="19" width="9.125" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="1"/>
@@ -587,7 +583,7 @@
         <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="128.25" x14ac:dyDescent="0.2">
@@ -597,14 +593,16 @@
       <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="1" t="str">
+        <f>_xlfn.CONCAT($B3,".",$C3,".",D$2)</f>
+        <v>Eula.Attack.Name</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f>_xlfn.CONCAT($B3,".",$C3,".",E$2)</f>
+        <v>Eula.Attack.Description</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -785,7 +783,7 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>